<commit_message>
feat: adds default buckets
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -1,39 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon.young\Projects\aind-data-transfer-service\tests\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C99C58-03C3-4006-9A2A-4C5770DEFAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>acq_datetime</t>
+  </si>
+  <si>
+    <t>subject_id</t>
+  </si>
+  <si>
+    <t>modality0</t>
+  </si>
+  <si>
+    <t>modality0.source</t>
+  </si>
+  <si>
+    <t>modality1</t>
+  </si>
+  <si>
+    <t>modality1.source</t>
+  </si>
+  <si>
+    <t>behavior</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>behavior-videos</t>
+  </si>
+  <si>
+    <t>/allen/aind/stage/fake/dir</t>
+  </si>
+  <si>
+    <t>SmartSPIM</t>
+  </si>
+  <si>
+    <t>654321</t>
+  </si>
+  <si>
+    <t>SPIM</t>
+  </si>
+  <si>
+    <t>ecephys</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,82 +109,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -415,191 +413,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col min="1" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>platform</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>acq_datetime</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>subject_id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>s3_bucket</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>modality0</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>modality0.source</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>modality1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>modality1.source</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>behavior</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>45203.16666666666</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>aind-behavior-data</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>behavior-videos</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>behavior</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45203.166666666657</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SmartSPIM</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
         <v>44989.6875</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>654321</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aind-open-data</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SPIM</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ecephys</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>44956.79236111111</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>654321</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>aind-ephys-data</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ecephys</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>behavior-videos</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44956.792361111111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" sqref="A2:A20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E20 G2:G20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="D2:D20 F2:F20" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid s3_bucket." promptTitle="s3_bucket" prompt="Select a s3_bucket from the dropdown" type="list">
-      <formula1>"aind-ephys-data,aind-ophys-data,aind-behavior-data,aind-private-data"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: adds default buckets (#81)
* feat: adds default buckets

* feat: removes unused imports
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -1,39 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon.young\Projects\aind-data-transfer-service\tests\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C99C58-03C3-4006-9A2A-4C5770DEFAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>acq_datetime</t>
+  </si>
+  <si>
+    <t>subject_id</t>
+  </si>
+  <si>
+    <t>modality0</t>
+  </si>
+  <si>
+    <t>modality0.source</t>
+  </si>
+  <si>
+    <t>modality1</t>
+  </si>
+  <si>
+    <t>modality1.source</t>
+  </si>
+  <si>
+    <t>behavior</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>behavior-videos</t>
+  </si>
+  <si>
+    <t>/allen/aind/stage/fake/dir</t>
+  </si>
+  <si>
+    <t>SmartSPIM</t>
+  </si>
+  <si>
+    <t>654321</t>
+  </si>
+  <si>
+    <t>SPIM</t>
+  </si>
+  <si>
+    <t>ecephys</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,82 +109,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -415,191 +413,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col min="1" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>platform</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>acq_datetime</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>subject_id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>s3_bucket</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>modality0</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>modality0.source</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>modality1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>modality1.source</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>behavior</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>45203.16666666666</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>aind-behavior-data</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>behavior-videos</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>behavior</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45203.166666666657</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SmartSPIM</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
         <v>44989.6875</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>654321</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aind-open-data</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SPIM</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ecephys</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>44956.79236111111</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>654321</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>aind-ephys-data</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ecephys</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>behavior-videos</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>/allen/aind/stage/fake/dir</t>
-        </is>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44956.792361111111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" sqref="A2:A20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E20 G2:G20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="D2:D20 F2:F20" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid s3_bucket." promptTitle="s3_bucket" prompt="Select a s3_bucket from the dropdown" type="list">
-      <formula1>"aind-ephys-data,aind-ophys-data,aind-behavior-data,aind-private-data"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update unit tests and code cleanup
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -1,96 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon.young\Projects\aind-data-transfer-service\tests\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C99C58-03C3-4006-9A2A-4C5770DEFAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>acq_datetime</t>
-  </si>
-  <si>
-    <t>subject_id</t>
-  </si>
-  <si>
-    <t>modality0</t>
-  </si>
-  <si>
-    <t>modality0.source</t>
-  </si>
-  <si>
-    <t>modality1</t>
-  </si>
-  <si>
-    <t>modality1.source</t>
-  </si>
-  <si>
-    <t>behavior</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>behavior-videos</t>
-  </si>
-  <si>
-    <t>/allen/aind/stage/fake/dir</t>
-  </si>
-  <si>
-    <t>SmartSPIM</t>
-  </si>
-  <si>
-    <t>654321</t>
-  </si>
-  <si>
-    <t>SPIM</t>
-  </si>
-  <si>
-    <t>ecephys</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -109,23 +53,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,112 +416,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45203.166666666657</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44989.6875</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44956.792361111111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>platform</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>acq_datetime</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>subject_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>modality0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>modality0.source</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>modality1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>modality1.source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>behavior</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="d">
+        <v>2023-10-04T04:00:00</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>behavior-videos</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>behavior</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SmartSPIM</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="d">
+        <v>2023-03-04T16:30:00</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>654321</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SPIM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ecephys</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="d">
+        <v>2023-01-30T19:01:00</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>654321</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ecephys</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>behavior-videos</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" sqref="A2:A20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="D2:D20 F2:F20" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation sqref="D2:D20 F2:F20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
     </dataValidation>
+    <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using yyyy-mm-dd hh:mm:ss" type="date"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update xlsx datetime format as YYYY-MM-DDTHH:mm:ss
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -18,7 +18,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DDTHH:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -626,7 +626,7 @@
     <dataValidation sqref="D2:D20 F2:F20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using yyyy-mm-dd hh:mm:ss" type="date"/>
+    <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" type="date"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Feat 85: validate & format datetime in xlsx job template (#87)
* add date validation for acq_datetime column

* enforce ISO 8601 datetime format for excel template

* update unit tests and code cleanup

* update xlsx datetime format as YYYY-MM-DDTHH:mm:ss
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -1,96 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon.young\Projects\aind-data-transfer-service\tests\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C99C58-03C3-4006-9A2A-4C5770DEFAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>acq_datetime</t>
-  </si>
-  <si>
-    <t>subject_id</t>
-  </si>
-  <si>
-    <t>modality0</t>
-  </si>
-  <si>
-    <t>modality0.source</t>
-  </si>
-  <si>
-    <t>modality1</t>
-  </si>
-  <si>
-    <t>modality1.source</t>
-  </si>
-  <si>
-    <t>behavior</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>behavior-videos</t>
-  </si>
-  <si>
-    <t>/allen/aind/stage/fake/dir</t>
-  </si>
-  <si>
-    <t>SmartSPIM</t>
-  </si>
-  <si>
-    <t>654321</t>
-  </si>
-  <si>
-    <t>SPIM</t>
-  </si>
-  <si>
-    <t>ecephys</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DDTHH:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -109,23 +53,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,112 +416,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45203.166666666657</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44989.6875</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44956.792361111111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>platform</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>acq_datetime</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>subject_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>modality0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>modality0.source</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>modality1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>modality1.source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>behavior</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="d">
+        <v>2023-10-04T04:00:00</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>behavior-videos</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>behavior</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SmartSPIM</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="d">
+        <v>2023-03-04T16:30:00</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>654321</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SPIM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ecephys</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="d">
+        <v>2023-01-30T19:01:00</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>654321</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ecephys</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>behavior-videos</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>/allen/aind/stage/fake/dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" sqref="A2:A20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="D2:D20 F2:F20" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation sqref="D2:D20 F2:F20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
     </dataValidation>
+    <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" type="date"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add metadata_dir to xlsx template in test/resources
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,7 @@
     <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,20 +457,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>metadata_dir</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>modality0</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>modality0.source</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>modality1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>modality1.source</t>
         </is>
@@ -491,20 +497,25 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>/allen/aind/stage/fake/metadata_dir</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>behavior-videos</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>behavior</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -526,10 +537,15 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>/allen/aind/stage/fake/Config</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>SPIM</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -549,22 +565,22 @@
           <t>654321</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>ecephys</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>behavior-videos</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -623,7 +639,7 @@
     <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D20 F2:F20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
+    <dataValidation sqref="E2:E20 G2:G20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" type="date"/>

</xml_diff>

<commit_message>
Feat 77: add metadata_dir field to excel template and validated jobs table (#88)
* Feat 77: add metadata_dir field to excel template and validated jobs table

* add metadata_dir to xlsx template in test/resources
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,7 @@
     <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,20 +457,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>metadata_dir</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>modality0</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>modality0.source</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>modality1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>modality1.source</t>
         </is>
@@ -491,20 +497,25 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>/allen/aind/stage/fake/metadata_dir</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>behavior-videos</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>behavior</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -526,10 +537,15 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>/allen/aind/stage/fake/Config</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>SPIM</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -549,22 +565,22 @@
           <t>654321</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>ecephys</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>behavior-videos</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -623,7 +639,7 @@
     <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D20 F2:F20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
+    <dataValidation sqref="E2:E20 G2:G20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" type="date"/>

</xml_diff>

<commit_message>
feat: adds new fields to template
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,45 +437,63 @@
     <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="13" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="13" bestFit="1" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>processor_full_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>process_capsule_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>platform</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>acq_datetime</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>subject_id</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>metadata_dir</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>modality0</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>modality0.source</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>modality1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>modality1.source</t>
         </is>
@@ -484,38 +502,53 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Anna Apple</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Behavior Platform</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1f999652-00a0-4c4b-99b5-64c2985ad070</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>behavior</t>
         </is>
       </c>
-      <c r="B2" s="2" t="d">
+      <c r="E2" s="2" t="d">
         <v>2023-10-04T04:00:00</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>123456</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/metadata_dir</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>behavior-videos</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>behavior</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -524,28 +557,38 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ophys Platform - SLAP2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>SmartSPIM</t>
         </is>
       </c>
-      <c r="B3" s="2" t="d">
+      <c r="E3" s="2" t="d">
         <v>2023-03-04T16:30:00</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>654321</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/Config</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>SPIM</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
@@ -554,95 +597,108 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Anna Apple</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ephys Platform</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>ecephys</t>
         </is>
       </c>
-      <c r="B4" s="2" t="d">
+      <c r="E4" s="2" t="d">
         <v>2023-01-30T19:01:00</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>654321</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>ecephys</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>behavior-videos</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>/allen/aind/stage/fake/dir</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="2" t="n"/>
+      <c r="E18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="A2:A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
+  <dataValidations count="4">
+    <dataValidation sqref="D2:D20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid platform." promptTitle="platform" prompt="Select a platform from the dropdown" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E20 G2:G20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
+    <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid project_name." promptTitle="project_name" prompt="Select a project_name from the dropdown" type="list">
+      <formula1>"AIND Viral Genetic Tools,Behavior Platform,Brain Computer Interface,Cell Type LUT,Cognitive flexibility in patch foraging,Discovery-Brain Wide Circuit Dynamics,Discovery-Neuromodulator circuit dynamics during foraging,Dynamic Routing,Ephys Platform,Force Foraging,Information seeking in partially observable environments,Learning mFISH/V1omFISH,MSMA Platform,Medulla,Neurobiology of Action,OpenScope,Ophys Platform - FP and indicator testing,Ophys Platform - SLAP2,Single-neuron computations within brain-wide circuits (SCBC),Thalamus in the middle"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H20 J2:J20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
     </dataValidation>
-    <dataValidation sqref="B2:B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" type="date"/>
+    <dataValidation sqref="E2:E20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" error="Invalid datetime." promptTitle="datetime" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" type="date"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: removes processor_full_name (#100)
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">processor_full_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve">project_name</t>
   </si>
@@ -55,9 +52,6 @@
     <t xml:space="preserve">modality1.source</t>
   </si>
   <si>
-    <t xml:space="preserve">Anna Apple</t>
-  </si>
-  <si>
     <t xml:space="preserve">Behavior Platform</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">/allen/aind/stage/fake/dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Smith</t>
   </si>
   <si>
     <t xml:space="preserve">Ophys Platform - SLAP2</t>
@@ -218,18 +209,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -260,212 +252,200 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="3" t="n">
+        <v>45203.1666666667</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>45203.1666666667</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>18</v>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>44989.6875</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="n">
-        <v>44989.6875</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="2"/>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>44956.7923611111</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="H12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="H13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="H15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="G5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="G18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="G20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" error="Invalid platform." errorStyle="stop" operator="between" prompt="Select a platform from the dropdown" promptTitle="platform" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D20" type="list">
+    <dataValidation allowBlank="true" error="Invalid platform." errorStyle="stop" operator="between" prompt="Select a platform from the dropdown" promptTitle="platform" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C20" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid project_name." errorStyle="stop" operator="between" prompt="Select a project_name from the dropdown" promptTitle="project_name" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B5:B20" type="list">
+    <dataValidation allowBlank="true" error="Invalid project_name." errorStyle="stop" operator="between" prompt="Select a project_name from the dropdown" promptTitle="project_name" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A5:A20" type="list">
       <formula1>"AIND Viral Genetic Tools,Behavior Platform,Brain Computer Interface,Cell Type LUT,Cognitive flexibility in patch foraging,Discovery-Brain Wide Circuit Dynamics,Discovery-Neuromodulator circuit dynamics during foraging,Dynamic Routing,Ephys Platform,Force "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid modality." errorStyle="stop" operator="between" prompt="Select a modality from the dropdown" promptTitle="modality" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H20 J2:J20" type="list">
+    <dataValidation allowBlank="true" error="Invalid modality." errorStyle="stop" operator="between" prompt="Select a modality from the dropdown" promptTitle="modality" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G20 I2:I20" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid datetime." errorStyle="stop" operator="between" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" promptTitle="datetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E20" type="date">
+    <dataValidation allowBlank="true" error="Invalid datetime." errorStyle="stop" operator="between" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" promptTitle="datetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D20" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
feat: adds input data mount field
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t xml:space="preserve">project_name</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">process_capsule_id</t>
   </si>
   <si>
+    <t xml:space="preserve">input_data_mount</t>
+  </si>
+  <si>
     <t xml:space="preserve">platform</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">1f999652-00a0-4c4b-99b5-64c2985ad070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_mount</t>
   </si>
   <si>
     <t xml:space="preserve">behavior</t>
@@ -209,16 +215,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,188 +257,194 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="n">
         <v>45203.1666666667</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>16</v>
+      <c r="K2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>44989.6875</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>44989.6875</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <v>44956.7923611111</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>16</v>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="G5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="G6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="G7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="H12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="G13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="H13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="G14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
+      <c r="H14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="H15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="G16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="H16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="H17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="H19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" error="Invalid platform." errorStyle="stop" operator="between" prompt="Select a platform from the dropdown" promptTitle="platform" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C20" type="list">
+    <dataValidation allowBlank="true" error="Invalid platform." errorStyle="stop" operator="between" prompt="Select a platform from the dropdown" promptTitle="platform" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D20" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -441,11 +452,11 @@
       <formula1>"AIND Viral Genetic Tools,Behavior Platform,Brain Computer Interface,Cell Type LUT,Cognitive flexibility in patch foraging,Discovery-Brain Wide Circuit Dynamics,Discovery-Neuromodulator circuit dynamics during foraging,Dynamic Routing,Ephys Platform,Force "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid modality." errorStyle="stop" operator="between" prompt="Select a modality from the dropdown" promptTitle="modality" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G20 I2:I20" type="list">
+    <dataValidation allowBlank="true" error="Invalid modality." errorStyle="stop" operator="between" prompt="Select a modality from the dropdown" promptTitle="modality" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H20 J2:J20" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid datetime." errorStyle="stop" operator="between" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" promptTitle="datetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D20" type="date">
+    <dataValidation allowBlank="true" error="Invalid datetime." errorStyle="stop" operator="between" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" promptTitle="datetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E20" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
feat: adds input data mount field (#116)
* feat: adds input data mount field
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t xml:space="preserve">project_name</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">process_capsule_id</t>
   </si>
   <si>
+    <t xml:space="preserve">input_data_mount</t>
+  </si>
+  <si>
     <t xml:space="preserve">platform</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">1f999652-00a0-4c4b-99b5-64c2985ad070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_mount</t>
   </si>
   <si>
     <t xml:space="preserve">behavior</t>
@@ -209,16 +215,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,188 +257,194 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="n">
         <v>45203.1666666667</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>16</v>
+      <c r="K2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>44989.6875</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>44989.6875</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <v>44956.7923611111</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>16</v>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="G5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="G6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="G7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="H12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="G13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="H13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="G14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
+      <c r="H14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="H15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="G16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="H16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="H17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="H19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" error="Invalid platform." errorStyle="stop" operator="between" prompt="Select a platform from the dropdown" promptTitle="platform" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C20" type="list">
+    <dataValidation allowBlank="true" error="Invalid platform." errorStyle="stop" operator="between" prompt="Select a platform from the dropdown" promptTitle="platform" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D20" type="list">
       <formula1>"behavior,confocal,ecephys,exaSPIM,FIP,HCR,HSFP,ISI,mesoSPIM,MERFISH,MRI,multiplane-ophys,single-plane-ophys,SLAP2,SmartSPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -441,11 +452,11 @@
       <formula1>"AIND Viral Genetic Tools,Behavior Platform,Brain Computer Interface,Cell Type LUT,Cognitive flexibility in patch foraging,Discovery-Brain Wide Circuit Dynamics,Discovery-Neuromodulator circuit dynamics during foraging,Dynamic Routing,Ephys Platform,Force "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid modality." errorStyle="stop" operator="between" prompt="Select a modality from the dropdown" promptTitle="modality" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G20 I2:I20" type="list">
+    <dataValidation allowBlank="true" error="Invalid modality." errorStyle="stop" operator="between" prompt="Select a modality from the dropdown" promptTitle="modality" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H20 J2:J20" type="list">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid datetime." errorStyle="stop" operator="between" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" promptTitle="datetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D20" type="date">
+    <dataValidation allowBlank="true" error="Invalid datetime." errorStyle="stop" operator="between" prompt="Provide a datetime using YYYY-MM-DDTHH:mm:ss" promptTitle="datetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E20" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
tests: update template in test
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helen.lin\Repos\aind-data-transfer-service\tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon.young\Projects\aind-data-transfer-service\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D14DA6-5C08-4954-8CB7-5221536A9A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BC1A7F-281C-465A-A831-546440611CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-21530" windowWidth="21820" windowHeight="37900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>project_name</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>modality1.input_source</t>
+  </si>
+  <si>
+    <t>derivatives_dir</t>
+  </si>
+  <si>
+    <t>/allen/aind/stage/fake/derivatives_dir</t>
   </si>
 </sst>
 </file>
@@ -479,18 +485,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="10" width="13" customWidth="1"/>
+    <col min="2" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -510,19 +516,22 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -542,19 +551,22 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -573,14 +585,14 @@
       <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -596,65 +608,65 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D20" s="2"/>
     </row>
   </sheetData>
@@ -667,7 +679,7 @@
       <formula1>"AIND Viral Genetic Tools,Behavior Platform,Brain Computer Interface,Cell Type LUT,Cognitive flexibility in patch foraging,Discovery-Brain Wide Circuit Dynamics,Discovery-Neuromodulator circuit dynamics during foraging,Dynamic Routing,Ephys Platform,Force "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="G2:G20 I2:I20" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="H2:H20 J2:J20" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
docs: updates documenation for derivatives
</commit_message>
<xml_diff>
--- a/tests/resources/job_upload_template.xlsx
+++ b/tests/resources/job_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon.young\Projects\aind-data-transfer-service\tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helen.lin\Repos\aind-data-transfer-service\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BC1A7F-281C-465A-A831-546440611CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D14DA6-5C08-4954-8CB7-5221536A9A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-21530" windowWidth="21820" windowHeight="37900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>project_name</t>
   </si>
@@ -97,12 +97,6 @@
   </si>
   <si>
     <t>modality1.input_source</t>
-  </si>
-  <si>
-    <t>derivatives_dir</t>
-  </si>
-  <si>
-    <t>/allen/aind/stage/fake/derivatives_dir</t>
   </si>
 </sst>
 </file>
@@ -485,18 +479,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="13" customWidth="1"/>
+    <col min="2" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -516,22 +510,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -551,22 +542,19 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -585,14 +573,14 @@
       <c r="F3" t="s">
         <v>16</v>
       </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
       <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -608,65 +596,65 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
   </sheetData>
@@ -679,7 +667,7 @@
       <formula1>"AIND Viral Genetic Tools,Behavior Platform,Brain Computer Interface,Cell Type LUT,Cognitive flexibility in patch foraging,Discovery-Brain Wide Circuit Dynamics,Discovery-Neuromodulator circuit dynamics during foraging,Dynamic Routing,Ephys Platform,Force "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="H2:H20 J2:J20" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid modality." promptTitle="modality" prompt="Select a modality from the dropdown" sqref="G2:G20 I2:I20" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"behavior,behavior-videos,confocal,ecephys,EMG,fMOST,icephys,ISI,fib,merfish,MRI,ophys,slap,SPIM"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>